<commit_message>
Se calibro lector ocr
</commit_message>
<xml_diff>
--- a/Celdas.xlsx
+++ b/Celdas.xlsx
@@ -424,433 +424,658 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Artículo nP Descripción Cant. Precio por unidad Descuento Precio</t>
+          <t>Artículo n</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Descripción</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cant.</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Precio por unidad</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Descuento</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Precio</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>24567</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 1</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5,00 €</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>195,00 €</t>
-        </is>
-      </c>
+          <t>1,00 €</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1,00 €</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Z4568</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 2</t>
+          <t>Factura 3-456 Datos 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4,00 €</t>
+          <t>2,00 €</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5,00 €</t>
+          <t>2,00 €</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>155,00 €</t>
+          <t>2,00 €</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>24569</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 3</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
+          <t>3,00 €</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3,00 €</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>6,00 €</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>7,00 €</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>173,00 €</t>
-        </is>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>24570</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7,00 €</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>4,00 €</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>4,00 €</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>280,00 €</t>
+          <t>12,00 €</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>24571</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 5</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4,00 €</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>5,00 €</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5,00 €</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>40,00 €</t>
+          <t>20,00 €</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>24572</t>
-        </is>
-      </c>
+      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>8,00 €</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
+          <t>6,00 €</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>6,00 €</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>40,00 €</t>
+          <t>30,00 €</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>24573</t>
-        </is>
-      </c>
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6,00 €</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>7,00 €</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>7,00 €</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>420,00 €</t>
+          <t>42,00 €</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>24574</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 8</t>
+          <t>Factura 3-456 Datos 8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4,00 €</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>8,00 €</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>8,00 €</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>100,00 €</t>
+          <t>56,00 €</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>24575</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 9</t>
+          <t>Factura 3-456 Datos</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7,00 €</t>
+          <t>9,00 €</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3,00 €</t>
+          <t>9,00 €</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>32,00 €</t>
+          <t>72,00 €</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>24576</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 10</t>
+          <t>Factura 3-456 Datos 10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1,00 €</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
+          <t>10,00 €</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10,00 €</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>80,00 €</t>
+          <t>90,00 €</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>24577</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 11</t>
+          <t>Factura 3-456 Datos 11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7,00 €</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>11,00 €</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>11,00 €</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>455,00 €</t>
+          <t>110,00 €</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>24578</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Factura 3-456-2 Datos 12</t>
+          <t>Factura 3-456 Datos 12</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1,00 €</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>12,00 €</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12,00 €</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>44,00 €</t>
+          <t>132,00 €</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 13</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>13,00 €</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>13,00 €</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>156,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 14</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>14,00 €</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>14,00 €</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>182,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 15</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>15,00 €</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>15,00 €</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>210,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 16</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>16,00 €</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>16,00 €</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>240,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 17</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>17,00 €</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>17,00 €</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>272,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 18</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>18,00 €</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>18,00 €</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>306,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 19</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>19,00 €</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>19,00 €</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>342,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 20</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>20,00 €</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>20,00 €</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>380,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 21</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>21,00 €</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>21,00 €</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>420,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 22</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>22,00 €</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>22,00 €</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>462,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 23</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>23,00 €</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>23,00 €</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>506,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 24</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>24,00 €</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>24,00 €</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>552,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Factura 3-456 Datos 25</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>25,00 €</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>25,00 €</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>600,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
         <is>
           <t>Subtotal de la factura</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>2.014,00 €</t>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>5.200,00 €</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
         <is>
           <t>Tipo impositivo</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>8,75%</t>
         </is>
@@ -864,7 +1089,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>176,23 €</t>
+          <t>455,00 €</t>
         </is>
       </c>
     </row>
@@ -874,7 +1099,11 @@
           <t>Otros</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>100,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -882,12 +1111,21 @@
           <t>Depósito recibido</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>100,00 €</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TOTAL 2.190,23 €</t>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>5.655,00 €</t>
         </is>
       </c>
     </row>

</xml_diff>